<commit_message>
Continuing to clean everything
</commit_message>
<xml_diff>
--- a/latex/stencils_content/stencils_benchmarks.xlsx
+++ b/latex/stencils_content/stencils_benchmarks.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23613"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="11700" yWindow="240" windowWidth="38720" windowHeight="28120" tabRatio="500" firstSheet="3" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="50420" windowHeight="28360" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Stencils RegularGrid" sheetId="5" r:id="rId1"/>
@@ -1118,6 +1118,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1659,6 +1660,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -1694,6 +1696,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -1707,6 +1710,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -4430,6 +4434,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -4671,6 +4676,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -4706,6 +4712,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -4719,6 +4726,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -4782,6 +4790,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -5010,6 +5019,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -5044,6 +5054,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -5057,6 +5068,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -5111,6 +5123,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -5555,6 +5568,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -5590,6 +5604,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -5603,6 +5618,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -8346,7 +8362,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
       <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
@@ -11905,7 +11921,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M39" sqref="M39"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Working toward completion in stencil generation
</commit_message>
<xml_diff>
--- a/latex/stencils_content/stencils_benchmarks.xlsx
+++ b/latex/stencils_content/stencils_benchmarks.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23613"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="50420" windowHeight="28360" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14980" tabRatio="500" firstSheet="6" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Stencils RegularGrid" sheetId="5" r:id="rId1"/>
@@ -235,8 +235,34 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="417">
+  <cellStyleXfs count="443">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -664,7 +690,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="417">
+  <cellStyles count="443">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -873,6 +899,19 @@
     <cellStyle name="Followed Hyperlink" xfId="412" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="414" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="416" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="418" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="420" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="422" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="424" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="426" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="428" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="430" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="432" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="434" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="436" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="438" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="440" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="442" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1081,6 +1120,19 @@
     <cellStyle name="Hyperlink" xfId="411" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="413" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="415" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="417" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="419" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="421" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="423" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="425" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="427" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="429" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="431" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="433" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="435" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="437" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="439" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="441" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1524,106 +1576,6 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="4"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Stencils RegularGrid'!$C$2</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>N</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'Stencils RegularGrid'!$C$3:$C$13</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>4000.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>8000.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>16000.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>32000.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>64000.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>128000.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>256000.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>512000.0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1.024E6</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2.048E6</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>4.096E6</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'Stencils RegularGrid'!$C$3:$C$13</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>4000.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>8000.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>16000.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>32000.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>64000.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>128000.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>256000.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>512000.0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1.024E6</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2.048E6</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>4.096E6</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -1632,11 +1584,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2143889016"/>
-        <c:axId val="-2118705112"/>
+        <c:axId val="2083353304"/>
+        <c:axId val="2083360344"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2143889016"/>
+        <c:axId val="2083353304"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -1667,12 +1619,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2118705112"/>
+        <c:crossAx val="2083360344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2118705112"/>
+        <c:axId val="2083360344"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -1703,7 +1655,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2143889016"/>
+        <c:crossAx val="2083353304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1939,11 +1891,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2116297896"/>
-        <c:axId val="-2091815544"/>
+        <c:axId val="2110649144"/>
+        <c:axId val="2110652136"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2116297896"/>
+        <c:axId val="2110649144"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -1955,12 +1907,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2091815544"/>
+        <c:crossAx val="2110652136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2091815544"/>
+        <c:axId val="2110652136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.75"/>
@@ -1972,13 +1924,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2116297896"/>
+        <c:crossAx val="2110649144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2023,6 +1976,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2215,11 +2169,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2094668744"/>
-        <c:axId val="-2115629256"/>
+        <c:axId val="2110693768"/>
+        <c:axId val="2110699240"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2094668744"/>
+        <c:axId val="2110693768"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -2243,18 +2197,19 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2115629256"/>
+        <c:crossAx val="2110699240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2115629256"/>
+        <c:axId val="2110699240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2277,19 +2232,21 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2094668744"/>
+        <c:crossAx val="2110693768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2454,11 +2411,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2088977992"/>
-        <c:axId val="-2119170840"/>
+        <c:axId val="2110739240"/>
+        <c:axId val="2110742232"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2088977992"/>
+        <c:axId val="2110739240"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -2469,12 +2426,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2119170840"/>
+        <c:crossAx val="2110742232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2119170840"/>
+        <c:axId val="2110742232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2485,13 +2442,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2088977992"/>
+        <c:crossAx val="2110739240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2658,11 +2616,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2142385544"/>
-        <c:axId val="-2089122008"/>
+        <c:axId val="2109777144"/>
+        <c:axId val="2109774152"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2142385544"/>
+        <c:axId val="2109777144"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -2673,12 +2631,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2089122008"/>
+        <c:crossAx val="2109774152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2089122008"/>
+        <c:axId val="2109774152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2689,13 +2647,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2142385544"/>
+        <c:crossAx val="2109777144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2826,11 +2785,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2116856472"/>
-        <c:axId val="-2116832680"/>
+        <c:axId val="2109746856"/>
+        <c:axId val="2109743864"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2116856472"/>
+        <c:axId val="2109746856"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -2841,12 +2800,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2116832680"/>
+        <c:crossAx val="2109743864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2116832680"/>
+        <c:axId val="2109743864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2857,7 +2816,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2116856472"/>
+        <c:crossAx val="2109746856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2917,6 +2876,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -3257,11 +3217,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2091071304"/>
-        <c:axId val="-2120909816"/>
+        <c:axId val="2122403768"/>
+        <c:axId val="2122409384"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2091071304"/>
+        <c:axId val="2122403768"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -3285,18 +3245,19 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2120909816"/>
+        <c:crossAx val="2122409384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2120909816"/>
+        <c:axId val="2122409384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3319,19 +3280,21 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2091071304"/>
+        <c:crossAx val="2122403768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3403,6 +3366,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -3743,11 +3707,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2116220280"/>
-        <c:axId val="-2124107592"/>
+        <c:axId val="2122456152"/>
+        <c:axId val="2122461768"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2116220280"/>
+        <c:axId val="2122456152"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -3771,18 +3735,19 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2124107592"/>
+        <c:crossAx val="2122461768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2124107592"/>
+        <c:axId val="2122461768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3805,19 +3770,21 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2116220280"/>
+        <c:crossAx val="2122456152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -4013,11 +3980,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2119432872"/>
-        <c:axId val="-2145972424"/>
+        <c:axId val="2122497416"/>
+        <c:axId val="2122502824"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2119432872"/>
+        <c:axId val="2122497416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="220.0"/>
@@ -4048,12 +4015,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2145972424"/>
+        <c:crossAx val="2122502824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2145972424"/>
+        <c:axId val="2122502824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4083,7 +4050,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2119432872"/>
+        <c:crossAx val="2122497416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4281,11 +4248,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2124956072"/>
-        <c:axId val="-2143792760"/>
+        <c:axId val="2122532952"/>
+        <c:axId val="2122538360"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2124956072"/>
+        <c:axId val="2122532952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="220.0"/>
@@ -4316,12 +4283,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2143792760"/>
+        <c:crossAx val="2122538360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2143792760"/>
+        <c:axId val="2122538360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="1.0"/>
@@ -4352,7 +4319,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2124956072"/>
+        <c:crossAx val="2122532952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4648,11 +4615,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2146902008"/>
-        <c:axId val="-2123643048"/>
+        <c:axId val="2087130312"/>
+        <c:axId val="2087135800"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2146902008"/>
+        <c:axId val="2087130312"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -4683,12 +4650,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2123643048"/>
+        <c:crossAx val="2087135800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2123643048"/>
+        <c:axId val="2087135800"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -4719,7 +4686,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2146902008"/>
+        <c:crossAx val="2087130312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4991,11 +4958,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2121473160"/>
-        <c:axId val="-2089316088"/>
+        <c:axId val="2087168248"/>
+        <c:axId val="2087173688"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2121473160"/>
+        <c:axId val="2087168248"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -5026,12 +4993,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2089316088"/>
+        <c:crossAx val="2087173688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2089316088"/>
+        <c:axId val="2087173688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5061,7 +5028,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2121473160"/>
+        <c:crossAx val="2087168248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5432,106 +5399,6 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Stencils RegularGrid'!$C$2</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>N</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'Stencils RegularGrid'!$C$3:$C$13</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>4000.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>8000.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>16000.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>32000.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>64000.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>128000.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>256000.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>512000.0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1.024E6</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2.048E6</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>4.096E6</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'Stencils RegularGrid'!$C$3:$C$13</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>4000.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>8000.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>16000.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>32000.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>64000.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>128000.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>256000.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>512000.0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1.024E6</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2.048E6</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>4.096E6</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -5540,11 +5407,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2094845800"/>
-        <c:axId val="-2094588488"/>
+        <c:axId val="2087215448"/>
+        <c:axId val="2087220984"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2094845800"/>
+        <c:axId val="2087215448"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -5575,12 +5442,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2094588488"/>
+        <c:crossAx val="2087220984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2094588488"/>
+        <c:axId val="2087220984"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -5611,7 +5478,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2094845800"/>
+        <c:crossAx val="2087215448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5673,6 +5540,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -5877,11 +5745,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2091166232"/>
-        <c:axId val="-2089198056"/>
+        <c:axId val="2087271768"/>
+        <c:axId val="2087277256"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2091166232"/>
+        <c:axId val="2087271768"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -5905,18 +5773,19 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2089198056"/>
+        <c:crossAx val="2087277256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2089198056"/>
+        <c:axId val="2087277256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5939,19 +5808,21 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2091166232"/>
+        <c:crossAx val="2087271768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -6015,6 +5886,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -6215,11 +6087,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2090945240"/>
-        <c:axId val="-2126916136"/>
+        <c:axId val="2087312104"/>
+        <c:axId val="2087317544"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2090945240"/>
+        <c:axId val="2087312104"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -6243,18 +6115,19 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2126916136"/>
+        <c:crossAx val="2087317544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2126916136"/>
+        <c:axId val="2087317544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6277,19 +6150,21 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2090945240"/>
+        <c:crossAx val="2087312104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -6344,6 +6219,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -6560,11 +6436,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2116471656"/>
-        <c:axId val="-2091747512"/>
+        <c:axId val="2111918264"/>
+        <c:axId val="2111926664"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2116471656"/>
+        <c:axId val="2111918264"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -6573,18 +6449,19 @@
         <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2091747512"/>
+        <c:crossAx val="2111926664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2091747512"/>
+        <c:axId val="2111926664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.2"/>
@@ -6594,19 +6471,21 @@
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:title>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2116471656"/>
+        <c:crossAx val="2111918264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -6661,6 +6540,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -6933,86 +6813,6 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:v>N</c:v>
-          </c:tx>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'Stencils Sphere'!$C$4:$C$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>4000.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>8000.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>16000.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>32000.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>64000.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>128000.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>256000.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>512000.0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>992000.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'Stencils Sphere'!$C$4:$C$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>4000.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>8000.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>16000.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>32000.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>64000.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>128000.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>256000.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>512000.0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>992000.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -7021,11 +6821,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2119324248"/>
-        <c:axId val="-2118414648"/>
+        <c:axId val="2110564264"/>
+        <c:axId val="2110569816"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2119324248"/>
+        <c:axId val="2110564264"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -7049,18 +6849,19 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2118414648"/>
+        <c:crossAx val="2110569816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2118414648"/>
+        <c:axId val="2110569816"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -7084,19 +6885,21 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2119324248"/>
+        <c:crossAx val="2110564264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -7151,6 +6954,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -7343,11 +7147,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2121576472"/>
-        <c:axId val="-2089341288"/>
+        <c:axId val="2110602712"/>
+        <c:axId val="2110608168"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2121576472"/>
+        <c:axId val="2110602712"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -7371,18 +7175,19 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2089341288"/>
+        <c:crossAx val="2110608168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2089341288"/>
+        <c:axId val="2110608168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7405,19 +7210,21 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2121576472"/>
+        <c:crossAx val="2110602712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -8362,8 +8169,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="H33" sqref="H33"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -8449,15 +8256,15 @@
         <v>84.918999999999997</v>
       </c>
       <c r="I3">
-        <f t="shared" ref="I3:I13" si="1">F3/D3</f>
+        <f>F3/D3</f>
         <v>1.015954847303008</v>
       </c>
       <c r="J3">
-        <f t="shared" ref="J3:J13" si="2">G3/D3</f>
+        <f>G3/D3</f>
         <v>0.81373554241689583</v>
       </c>
       <c r="K3">
-        <f t="shared" ref="K3:K13" si="3">G3/E3</f>
+        <f>G3/E3</f>
         <v>0.44472084169071319</v>
       </c>
     </row>
@@ -8482,15 +8289,15 @@
         <v>181.43600000000001</v>
       </c>
       <c r="I4">
-        <f t="shared" si="1"/>
+        <f>F4/D4</f>
         <v>1.312855037799513</v>
       </c>
       <c r="J4">
-        <f t="shared" si="2"/>
+        <f>G4/D4</f>
         <v>0.96867125101439377</v>
       </c>
       <c r="K4">
-        <f t="shared" si="3"/>
+        <f>G4/E4</f>
         <v>0.51694850060545616</v>
       </c>
     </row>
@@ -8515,15 +8322,15 @@
         <v>444.61799999999999</v>
       </c>
       <c r="I5">
-        <f t="shared" si="1"/>
+        <f>F5/D5</f>
         <v>1.8755694876438438</v>
       </c>
       <c r="J5">
-        <f t="shared" si="2"/>
+        <f>G5/D5</f>
         <v>1.2035862494619813</v>
       </c>
       <c r="K5">
-        <f t="shared" si="3"/>
+        <f>G5/E5</f>
         <v>0.63213882036809288</v>
       </c>
     </row>
@@ -8548,15 +8355,15 @@
         <v>1007.2809999999999</v>
       </c>
       <c r="I6">
-        <f t="shared" si="1"/>
+        <f>F6/D6</f>
         <v>3.7943915967486976</v>
       </c>
       <c r="J6">
-        <f t="shared" si="2"/>
+        <f>G6/D6</f>
         <v>1.8843355688376313</v>
       </c>
       <c r="K6">
-        <f t="shared" si="3"/>
+        <f>G6/E6</f>
         <v>0.43876950384221319</v>
       </c>
     </row>
@@ -8581,15 +8388,15 @@
         <v>2062.9861000000001</v>
       </c>
       <c r="I7">
-        <f t="shared" si="1"/>
+        <f>F7/D7</f>
         <v>5.372125840362572</v>
       </c>
       <c r="J7">
-        <f t="shared" si="2"/>
+        <f>G7/D7</f>
         <v>1.8282692386089108</v>
       </c>
       <c r="K7">
-        <f t="shared" si="3"/>
+        <f>G7/E7</f>
         <v>0.33128476566382897</v>
       </c>
     </row>
@@ -8614,15 +8421,15 @@
         <v>4309.2349000000004</v>
       </c>
       <c r="I8">
-        <f t="shared" si="1"/>
+        <f>F8/D8</f>
         <v>9.4502344674259628</v>
       </c>
       <c r="J8">
-        <f t="shared" si="2"/>
+        <f>G8/D8</f>
         <v>1.9859955083645535</v>
       </c>
       <c r="K8">
-        <f t="shared" si="3"/>
+        <f>G8/E8</f>
         <v>0.32812641819944399</v>
       </c>
     </row>
@@ -8647,15 +8454,15 @@
         <v>8680.1767999999993</v>
       </c>
       <c r="I9">
-        <f t="shared" si="1"/>
+        <f>F9/D9</f>
         <v>16.85035838544448</v>
       </c>
       <c r="J9">
-        <f t="shared" si="2"/>
+        <f>G9/D9</f>
         <v>2.006701599516663</v>
       </c>
       <c r="K9">
-        <f t="shared" si="3"/>
+        <f>G9/E9</f>
         <v>0.32007840197637449</v>
       </c>
     </row>
@@ -8680,15 +8487,15 @@
         <v>17348.968799999999</v>
       </c>
       <c r="I10">
-        <f t="shared" si="1"/>
+        <f>F10/D10</f>
         <v>31.047931881705914</v>
       </c>
       <c r="J10">
-        <f t="shared" si="2"/>
+        <f>G10/D10</f>
         <v>1.9644716804971805</v>
       </c>
       <c r="K10">
-        <f t="shared" si="3"/>
+        <f>G10/E10</f>
         <v>0.3058119720037476</v>
       </c>
     </row>
@@ -8713,15 +8520,15 @@
         <v>31436.804700000001</v>
       </c>
       <c r="I11">
-        <f t="shared" si="1"/>
+        <f>F11/D11</f>
         <v>59.660523122362761</v>
       </c>
       <c r="J11">
-        <f t="shared" si="2"/>
+        <f>G11/D11</f>
         <v>1.77441265811326</v>
       </c>
       <c r="K11">
-        <f t="shared" si="3"/>
+        <f>G11/E11</f>
         <v>0.25524188299909928</v>
       </c>
     </row>
@@ -8746,15 +8553,15 @@
         <v>54543.167999999998</v>
       </c>
       <c r="I12">
-        <f t="shared" si="1"/>
+        <f>F12/D12</f>
         <v>117.68715871679784</v>
       </c>
       <c r="J12">
-        <f t="shared" si="2"/>
+        <f>G12/D12</f>
         <v>1.5288265363711961</v>
       </c>
       <c r="K12">
-        <f t="shared" si="3"/>
+        <f>G12/E12</f>
         <v>0.21472396362270507</v>
       </c>
     </row>
@@ -8776,15 +8583,15 @@
         <v>100177.25</v>
       </c>
       <c r="I13">
-        <f t="shared" si="1"/>
+        <f>F13/D13</f>
         <v>0</v>
       </c>
       <c r="J13">
-        <f t="shared" si="2"/>
+        <f>G13/D13</f>
         <v>1.3996294051795952</v>
       </c>
       <c r="K13">
-        <f t="shared" si="3"/>
+        <f>G13/E13</f>
         <v>0.19108633503496653</v>
       </c>
     </row>
@@ -8818,7 +8625,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A32" workbookViewId="0">
       <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
@@ -9250,7 +9057,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A24" workbookViewId="0">
       <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
@@ -9683,7 +9490,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:I12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A69" workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
@@ -9959,7 +9766,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:I12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A35" workbookViewId="0">
       <selection activeCell="O43" sqref="O43"/>
     </sheetView>
   </sheetViews>
@@ -10235,7 +10042,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:I11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A27" workbookViewId="0">
       <selection activeCell="I51" sqref="I51"/>
     </sheetView>
   </sheetViews>
@@ -10523,7 +10330,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:X17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A42" workbookViewId="0">
       <selection activeCell="O27" sqref="O27"/>
     </sheetView>
   </sheetViews>
@@ -11508,7 +11315,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="J60" sqref="J60"/>
     </sheetView>
   </sheetViews>
@@ -11921,7 +11728,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="M39" sqref="M39"/>
     </sheetView>
   </sheetViews>
@@ -12003,27 +11810,27 @@
         <v>44</v>
       </c>
       <c r="B7">
-        <f>B6/64000</f>
+        <f t="shared" ref="B7:G7" si="0">B6/64000</f>
         <v>0.15828665156249999</v>
       </c>
       <c r="C7">
-        <f>C6/64000</f>
+        <f t="shared" si="0"/>
         <v>0.14954502812499998</v>
       </c>
       <c r="D7">
-        <f>D6/64000</f>
+        <f t="shared" si="0"/>
         <v>0.14892755156250001</v>
       </c>
       <c r="E7">
-        <f>E6/64000</f>
+        <f t="shared" si="0"/>
         <v>0.15065772968749999</v>
       </c>
       <c r="F7">
-        <f>F6/64000</f>
+        <f t="shared" si="0"/>
         <v>0.14905113281249999</v>
       </c>
       <c r="G7">
-        <f>G6/64000</f>
+        <f t="shared" si="0"/>
         <v>0.14991095000000002</v>
       </c>
     </row>
@@ -12032,27 +11839,27 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <f>$B$7/B7</f>
+        <f t="shared" ref="B8:G8" si="1">$B$7/B7</f>
         <v>1</v>
       </c>
       <c r="C8">
-        <f>$B$7/C7</f>
+        <f t="shared" si="1"/>
         <v>1.0584547914905815</v>
       </c>
       <c r="D8">
-        <f>$B$7/D7</f>
+        <f t="shared" si="1"/>
         <v>1.0628433080501714</v>
       </c>
       <c r="E8">
-        <f>$B$7/E7</f>
+        <f t="shared" si="1"/>
         <v>1.0506374408457118</v>
       </c>
       <c r="F8">
-        <f>$B$7/F7</f>
+        <f t="shared" si="1"/>
         <v>1.0619620835865629</v>
       </c>
       <c r="G8">
-        <f>$B$7/G7</f>
+        <f t="shared" si="1"/>
         <v>1.0558711792734286</v>
       </c>
     </row>
@@ -12114,27 +11921,27 @@
         <v>6</v>
       </c>
       <c r="B14">
-        <f>$B$13/B13</f>
+        <f t="shared" ref="B14:G14" si="2">$B$13/B13</f>
         <v>1</v>
       </c>
       <c r="C14">
-        <f>$B$13/C13</f>
+        <f t="shared" si="2"/>
         <v>0.98871087533156488</v>
       </c>
       <c r="D14">
-        <f>$B$13/D13</f>
+        <f t="shared" si="2"/>
         <v>0.97240947511217779</v>
       </c>
       <c r="E14">
-        <f>$B$13/E13</f>
+        <f t="shared" si="2"/>
         <v>0.95330946291560104</v>
       </c>
       <c r="F14">
-        <f>$B$13/F13</f>
+        <f t="shared" si="2"/>
         <v>0.98630397967823868</v>
       </c>
       <c r="G14">
-        <f>$B$13/G13</f>
+        <f t="shared" si="2"/>
         <v>0.99039217770219989</v>
       </c>
     </row>
@@ -12197,27 +12004,27 @@
     </row>
     <row r="19" spans="1:9">
       <c r="B19">
-        <f>$B$18/B18</f>
+        <f t="shared" ref="B19:G19" si="3">$B$18/B18</f>
         <v>1</v>
       </c>
       <c r="C19">
-        <f>$B$18/C18</f>
+        <f t="shared" si="3"/>
         <v>1.2871078302135512</v>
       </c>
       <c r="D19">
-        <f>$B$18/D18</f>
+        <f t="shared" si="3"/>
         <v>0.12833859095688749</v>
       </c>
       <c r="E19">
-        <f>$B$18/E18</f>
+        <f t="shared" si="3"/>
         <v>9.1553521866326606E-2</v>
       </c>
       <c r="F19">
-        <f>$B$18/F18</f>
+        <f t="shared" si="3"/>
         <v>0.13242554114902622</v>
       </c>
       <c r="G19">
-        <f>$B$18/G18</f>
+        <f t="shared" si="3"/>
         <v>0.13620891691311868</v>
       </c>
     </row>
@@ -12298,15 +12105,15 @@
         <v>0.15313169900000001</v>
       </c>
       <c r="C34">
-        <f t="shared" ref="C34:E34" si="0">C33/100000</f>
+        <f t="shared" ref="C34:E34" si="4">C33/100000</f>
         <v>0.15077310499999999</v>
       </c>
       <c r="D34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0.15078171899999998</v>
       </c>
       <c r="E34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0.150381562</v>
       </c>
       <c r="F34">
@@ -12327,23 +12134,23 @@
         <v>1</v>
       </c>
       <c r="C35">
-        <f t="shared" ref="C35:G35" si="1">$B$34/C34</f>
+        <f t="shared" ref="C35:G35" si="5">$B$34/C34</f>
         <v>1.0156433337364779</v>
       </c>
       <c r="D35">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>1.0155853111079072</v>
       </c>
       <c r="E35">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>1.0182877273212525</v>
       </c>
       <c r="F35">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>1.0241404404997658</v>
       </c>
       <c r="G35">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>1.0197869640519728</v>
       </c>
     </row>
@@ -12409,23 +12216,23 @@
         <v>1</v>
       </c>
       <c r="C41">
-        <f t="shared" ref="C41:G41" si="2">$B$40/C40</f>
+        <f t="shared" ref="C41:G41" si="6">$B$40/C40</f>
         <v>1.0052651924127911</v>
       </c>
       <c r="D41">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1.0110196530552056</v>
       </c>
       <c r="E41">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0.9898411865074157</v>
       </c>
       <c r="F41">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1.0049704835894087</v>
       </c>
       <c r="G41">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1.0107621996166889</v>
       </c>
     </row>
@@ -12482,38 +12289,38 @@
     </row>
     <row r="46" spans="1:7">
       <c r="B46">
-        <f>$B$45/B45</f>
+        <f t="shared" ref="B46:G46" si="7">$B$45/B45</f>
         <v>1</v>
       </c>
       <c r="C46">
-        <f>$B$45/C45</f>
+        <f t="shared" si="7"/>
         <v>0.63277576505048949</v>
       </c>
       <c r="D46">
-        <f>$B$45/D45</f>
+        <f t="shared" si="7"/>
         <v>0.11138550048168903</v>
       </c>
       <c r="E46">
-        <f>$B$45/E45</f>
+        <f t="shared" si="7"/>
         <v>9.3302115181341849E-2</v>
       </c>
       <c r="F46">
-        <f>$B$45/F45</f>
+        <f t="shared" si="7"/>
         <v>0.11636544049897228</v>
       </c>
       <c r="G46">
-        <f>$B$45/G45</f>
+        <f t="shared" si="7"/>
         <v>0.11631927224292576</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="B43:G43"/>
     <mergeCell ref="B4:G4"/>
     <mergeCell ref="B11:G11"/>
     <mergeCell ref="B16:G16"/>
     <mergeCell ref="B31:G31"/>
     <mergeCell ref="B38:G38"/>
-    <mergeCell ref="B43:G43"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Almost done with chapter
</commit_message>
<xml_diff>
--- a/latex/stencils_content/stencils_benchmarks.xlsx
+++ b/latex/stencils_content/stencils_benchmarks.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23613"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14980" tabRatio="500" firstSheet="6" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="28420" tabRatio="500" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Stencils RegularGrid" sheetId="5" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="58">
   <si>
     <t xml:space="preserve">This is the regular grid. It is generated in raster order and is considered more or less ideal for generating the stencils. And yet we get 31x+ faster with the hash approach. </t>
   </si>
@@ -181,6 +181,27 @@
   <si>
     <t>100K CVT</t>
   </si>
+  <si>
+    <t>Nodes per Cell</t>
+  </si>
+  <si>
+    <t>Cell Count</t>
+  </si>
+  <si>
+    <t>exclude (0,1)</t>
+  </si>
+  <si>
+    <t>exclude (0)</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>MEAN</t>
+  </si>
+  <si>
+    <t>exclude (0, 1, 2)</t>
+  </si>
 </sst>
 </file>
 
@@ -235,8 +256,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="443">
+  <cellStyleXfs count="455">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -690,7 +723,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="443">
+  <cellStyles count="455">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -912,6 +945,12 @@
     <cellStyle name="Followed Hyperlink" xfId="438" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="440" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="442" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="444" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="446" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="448" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="450" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="452" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="454" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1133,6 +1172,12 @@
     <cellStyle name="Hyperlink" xfId="437" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="439" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="441" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="443" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="445" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="447" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="449" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="451" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="453" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1584,11 +1629,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2083353304"/>
-        <c:axId val="2083360344"/>
+        <c:axId val="-2120905608"/>
+        <c:axId val="-2120912552"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2083353304"/>
+        <c:axId val="-2120905608"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -1619,12 +1664,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2083360344"/>
+        <c:crossAx val="-2120912552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2083360344"/>
+        <c:axId val="-2120912552"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -1655,7 +1700,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2083353304"/>
+        <c:crossAx val="-2120905608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1891,11 +1936,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2110649144"/>
-        <c:axId val="2110652136"/>
+        <c:axId val="-2121226744"/>
+        <c:axId val="-2121229736"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2110649144"/>
+        <c:axId val="-2121226744"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -1907,12 +1952,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2110652136"/>
+        <c:crossAx val="-2121229736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2110652136"/>
+        <c:axId val="-2121229736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.75"/>
@@ -1924,7 +1969,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2110649144"/>
+        <c:crossAx val="-2121226744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2169,11 +2214,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2110693768"/>
-        <c:axId val="2110699240"/>
+        <c:axId val="-2118685432"/>
+        <c:axId val="-2118679992"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2110693768"/>
+        <c:axId val="-2118685432"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -2204,12 +2249,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2110699240"/>
+        <c:crossAx val="-2118679992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2110699240"/>
+        <c:axId val="-2118679992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2239,7 +2284,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2110693768"/>
+        <c:crossAx val="-2118685432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2411,11 +2456,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2110739240"/>
-        <c:axId val="2110742232"/>
+        <c:axId val="-2118640072"/>
+        <c:axId val="-2118637080"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2110739240"/>
+        <c:axId val="-2118640072"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -2426,12 +2471,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2110742232"/>
+        <c:crossAx val="-2118637080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2110742232"/>
+        <c:axId val="-2118637080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2442,7 +2487,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2110739240"/>
+        <c:crossAx val="-2118640072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2616,11 +2661,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2109777144"/>
-        <c:axId val="2109774152"/>
+        <c:axId val="-2118608824"/>
+        <c:axId val="-2118605832"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2109777144"/>
+        <c:axId val="-2118608824"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -2631,12 +2676,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2109774152"/>
+        <c:crossAx val="-2118605832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2109774152"/>
+        <c:axId val="-2118605832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2647,7 +2692,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2109777144"/>
+        <c:crossAx val="-2118608824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2785,11 +2830,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2109746856"/>
-        <c:axId val="2109743864"/>
+        <c:axId val="-2118578552"/>
+        <c:axId val="-2118575560"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2109746856"/>
+        <c:axId val="-2118578552"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -2800,12 +2845,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2109743864"/>
+        <c:crossAx val="-2118575560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2109743864"/>
+        <c:axId val="-2118575560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2816,7 +2861,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2109746856"/>
+        <c:crossAx val="-2118578552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3217,11 +3262,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2122403768"/>
-        <c:axId val="2122409384"/>
+        <c:axId val="-2118526040"/>
+        <c:axId val="-2118520424"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2122403768"/>
+        <c:axId val="-2118526040"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -3252,12 +3297,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2122409384"/>
+        <c:crossAx val="-2118520424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2122409384"/>
+        <c:axId val="-2118520424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3287,7 +3332,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2122403768"/>
+        <c:crossAx val="-2118526040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3707,11 +3752,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2122456152"/>
-        <c:axId val="2122461768"/>
+        <c:axId val="-2118473656"/>
+        <c:axId val="-2118468040"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2122456152"/>
+        <c:axId val="-2118473656"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -3742,12 +3787,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2122461768"/>
+        <c:crossAx val="-2118468040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2122461768"/>
+        <c:axId val="-2118468040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3777,7 +3822,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2122456152"/>
+        <c:crossAx val="-2118473656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3980,11 +4025,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2122497416"/>
-        <c:axId val="2122502824"/>
+        <c:axId val="-2118432568"/>
+        <c:axId val="-2118427160"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2122497416"/>
+        <c:axId val="-2118432568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="220.0"/>
@@ -4015,12 +4060,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2122502824"/>
+        <c:crossAx val="-2118427160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2122502824"/>
+        <c:axId val="-2118427160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4050,7 +4095,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2122497416"/>
+        <c:crossAx val="-2118432568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4248,11 +4293,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2122532952"/>
-        <c:axId val="2122538360"/>
+        <c:axId val="-2118397032"/>
+        <c:axId val="-2118391624"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2122532952"/>
+        <c:axId val="-2118397032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="220.0"/>
@@ -4283,12 +4328,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2122538360"/>
+        <c:crossAx val="-2118391624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2122538360"/>
+        <c:axId val="-2118391624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="1.0"/>
@@ -4319,7 +4364,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2122532952"/>
+        <c:crossAx val="-2118397032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4338,6 +4383,228 @@
       <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart19.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Variable HNX'!$D$63:$D$81</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>19.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>20.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Variable HNX'!$E$63:$E$81</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>409034.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44542.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>13669.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11480.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11780.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11422.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10341.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8518.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6077.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4037.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2271.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1190.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>552.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>243.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>86.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>38.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="-2119543096"/>
+        <c:axId val="-2094308648"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-2119543096"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2094308648"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2094308648"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2119543096"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
@@ -4615,11 +4882,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2087130312"/>
-        <c:axId val="2087135800"/>
+        <c:axId val="-2120982744"/>
+        <c:axId val="-2120988184"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2087130312"/>
+        <c:axId val="-2120982744"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -4650,12 +4917,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2087135800"/>
+        <c:crossAx val="-2120988184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2087135800"/>
+        <c:axId val="-2120988184"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -4686,7 +4953,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2087130312"/>
+        <c:crossAx val="-2120982744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4710,6 +4977,496 @@
       <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart20.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'Variable HNX'!$O$62:$O$124</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="63"/>
+                <c:pt idx="0">
+                  <c:v>93739.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>61732.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>32127.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15557.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7272.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3753.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1991.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1156.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>776.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>566.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>501.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>378.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>345.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>332.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>329.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>344.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>327.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>314.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>339.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>333.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>314.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>364.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>341.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>349.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>366.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>362.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>364.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>382.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>420.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>422.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>542.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>573.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>607.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>601.0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>641.0</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>632.0</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>647.0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>648.0</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>644.0</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>582.0</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>562.0</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>467.0</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>442.0</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>427.0</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>360.0</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>306.0</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>254.0</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>190.0</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>153.0</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>119.0</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>91.0</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>70.0</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>40.0</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>40.0</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>29.0</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>26.0</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>21.0</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>1.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'Variable HNX'!$P$62:$P$124</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="63"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>21.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>22.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>24.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>25.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>26.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>27.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>28.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>29.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>30.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>31.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>33.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>34.0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>35.0</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>36.0</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>37.0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>38.0</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>39.0</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>40.0</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>41.0</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>42.0</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>43.0</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>44.0</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>45.0</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>46.0</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>47.0</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>48.0</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>49.0</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>51.0</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>52.0</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>53.0</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>54.0</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>55.0</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>56.0</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>57.0</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>58.0</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>59.0</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>60.0</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>61.0</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>62.0</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>65.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="-2096978904"/>
+        <c:axId val="-2107683480"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-2096978904"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2107683480"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2107683480"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2096978904"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
@@ -4958,11 +5715,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2087168248"/>
-        <c:axId val="2087173688"/>
+        <c:axId val="-2121020808"/>
+        <c:axId val="-2121026248"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2087168248"/>
+        <c:axId val="-2121020808"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -4993,12 +5750,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2087173688"/>
+        <c:crossAx val="-2121026248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2087173688"/>
+        <c:axId val="-2121026248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5028,7 +5785,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2087168248"/>
+        <c:crossAx val="-2121020808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5407,11 +6164,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2087215448"/>
-        <c:axId val="2087220984"/>
+        <c:axId val="-2121063256"/>
+        <c:axId val="-2121068696"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2087215448"/>
+        <c:axId val="-2121063256"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -5442,12 +6199,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2087220984"/>
+        <c:crossAx val="-2121068696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2087220984"/>
+        <c:axId val="-2121068696"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -5478,7 +6235,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2087215448"/>
+        <c:crossAx val="-2121063256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5745,11 +6502,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2087271768"/>
-        <c:axId val="2087277256"/>
+        <c:axId val="-2119703704"/>
+        <c:axId val="-2119698232"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2087271768"/>
+        <c:axId val="-2119703704"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -5780,12 +6537,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2087277256"/>
+        <c:crossAx val="-2119698232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2087277256"/>
+        <c:axId val="-2119698232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5815,7 +6572,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2087271768"/>
+        <c:crossAx val="-2119703704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6087,11 +6844,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2087312104"/>
-        <c:axId val="2087317544"/>
+        <c:axId val="-2119663688"/>
+        <c:axId val="-2119658248"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2087312104"/>
+        <c:axId val="-2119663688"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -6122,12 +6879,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2087317544"/>
+        <c:crossAx val="-2119658248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2087317544"/>
+        <c:axId val="-2119658248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6157,7 +6914,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2087312104"/>
+        <c:crossAx val="-2119663688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6436,11 +7193,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2111918264"/>
-        <c:axId val="2111926664"/>
+        <c:axId val="-2119616680"/>
+        <c:axId val="-2121052008"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2111918264"/>
+        <c:axId val="-2119616680"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -6449,6 +7206,21 @@
         <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>N Stencils</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
           <c:layout/>
           <c:overlay val="0"/>
         </c:title>
@@ -6456,12 +7228,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2111926664"/>
+        <c:crossAx val="-2121052008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2111926664"/>
+        <c:axId val="-2121052008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.2"/>
@@ -6471,6 +7243,21 @@
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Speedup</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
           <c:layout/>
           <c:overlay val="0"/>
         </c:title>
@@ -6478,7 +7265,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2111918264"/>
+        <c:crossAx val="-2119616680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6821,11 +7608,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2110564264"/>
-        <c:axId val="2110569816"/>
+        <c:axId val="-2121140744"/>
+        <c:axId val="-2121146216"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2110564264"/>
+        <c:axId val="-2121140744"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -6856,12 +7643,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2110569816"/>
+        <c:crossAx val="-2121146216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2110569816"/>
+        <c:axId val="-2121146216"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -6892,7 +7679,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2110564264"/>
+        <c:crossAx val="-2121140744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7147,11 +7934,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2110602712"/>
-        <c:axId val="2110608168"/>
+        <c:axId val="-2121180280"/>
+        <c:axId val="-2121185720"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2110602712"/>
+        <c:axId val="-2121180280"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -7182,12 +7969,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2110608168"/>
+        <c:crossAx val="-2121185720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2110608168"/>
+        <c:axId val="-2121185720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7217,7 +8004,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2110602712"/>
+        <c:crossAx val="-2121180280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7842,6 +8629,66 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>520700</xdr:colOff>
+      <xdr:row>103</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>800100</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>88900</xdr:colOff>
+      <xdr:row>102</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Chart 7"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -8169,7 +9016,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
+    <sheetView topLeftCell="A46" workbookViewId="0">
       <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
@@ -8256,15 +9103,15 @@
         <v>84.918999999999997</v>
       </c>
       <c r="I3">
-        <f>F3/D3</f>
+        <f t="shared" ref="I3:I13" si="1">F3/D3</f>
         <v>1.015954847303008</v>
       </c>
       <c r="J3">
-        <f>G3/D3</f>
+        <f t="shared" ref="J3:J13" si="2">G3/D3</f>
         <v>0.81373554241689583</v>
       </c>
       <c r="K3">
-        <f>G3/E3</f>
+        <f t="shared" ref="K3:K13" si="3">G3/E3</f>
         <v>0.44472084169071319</v>
       </c>
     </row>
@@ -8289,15 +9136,15 @@
         <v>181.43600000000001</v>
       </c>
       <c r="I4">
-        <f>F4/D4</f>
+        <f t="shared" si="1"/>
         <v>1.312855037799513</v>
       </c>
       <c r="J4">
-        <f>G4/D4</f>
+        <f t="shared" si="2"/>
         <v>0.96867125101439377</v>
       </c>
       <c r="K4">
-        <f>G4/E4</f>
+        <f t="shared" si="3"/>
         <v>0.51694850060545616</v>
       </c>
     </row>
@@ -8322,15 +9169,15 @@
         <v>444.61799999999999</v>
       </c>
       <c r="I5">
-        <f>F5/D5</f>
+        <f t="shared" si="1"/>
         <v>1.8755694876438438</v>
       </c>
       <c r="J5">
-        <f>G5/D5</f>
+        <f t="shared" si="2"/>
         <v>1.2035862494619813</v>
       </c>
       <c r="K5">
-        <f>G5/E5</f>
+        <f t="shared" si="3"/>
         <v>0.63213882036809288</v>
       </c>
     </row>
@@ -8355,15 +9202,15 @@
         <v>1007.2809999999999</v>
       </c>
       <c r="I6">
-        <f>F6/D6</f>
+        <f t="shared" si="1"/>
         <v>3.7943915967486976</v>
       </c>
       <c r="J6">
-        <f>G6/D6</f>
+        <f t="shared" si="2"/>
         <v>1.8843355688376313</v>
       </c>
       <c r="K6">
-        <f>G6/E6</f>
+        <f t="shared" si="3"/>
         <v>0.43876950384221319</v>
       </c>
     </row>
@@ -8388,15 +9235,15 @@
         <v>2062.9861000000001</v>
       </c>
       <c r="I7">
-        <f>F7/D7</f>
+        <f t="shared" si="1"/>
         <v>5.372125840362572</v>
       </c>
       <c r="J7">
-        <f>G7/D7</f>
+        <f t="shared" si="2"/>
         <v>1.8282692386089108</v>
       </c>
       <c r="K7">
-        <f>G7/E7</f>
+        <f t="shared" si="3"/>
         <v>0.33128476566382897</v>
       </c>
     </row>
@@ -8421,15 +9268,15 @@
         <v>4309.2349000000004</v>
       </c>
       <c r="I8">
-        <f>F8/D8</f>
+        <f t="shared" si="1"/>
         <v>9.4502344674259628</v>
       </c>
       <c r="J8">
-        <f>G8/D8</f>
+        <f t="shared" si="2"/>
         <v>1.9859955083645535</v>
       </c>
       <c r="K8">
-        <f>G8/E8</f>
+        <f t="shared" si="3"/>
         <v>0.32812641819944399</v>
       </c>
     </row>
@@ -8454,15 +9301,15 @@
         <v>8680.1767999999993</v>
       </c>
       <c r="I9">
-        <f>F9/D9</f>
+        <f t="shared" si="1"/>
         <v>16.85035838544448</v>
       </c>
       <c r="J9">
-        <f>G9/D9</f>
+        <f t="shared" si="2"/>
         <v>2.006701599516663</v>
       </c>
       <c r="K9">
-        <f>G9/E9</f>
+        <f t="shared" si="3"/>
         <v>0.32007840197637449</v>
       </c>
     </row>
@@ -8487,15 +9334,15 @@
         <v>17348.968799999999</v>
       </c>
       <c r="I10">
-        <f>F10/D10</f>
+        <f t="shared" si="1"/>
         <v>31.047931881705914</v>
       </c>
       <c r="J10">
-        <f>G10/D10</f>
+        <f t="shared" si="2"/>
         <v>1.9644716804971805</v>
       </c>
       <c r="K10">
-        <f>G10/E10</f>
+        <f t="shared" si="3"/>
         <v>0.3058119720037476</v>
       </c>
     </row>
@@ -8520,15 +9367,15 @@
         <v>31436.804700000001</v>
       </c>
       <c r="I11">
-        <f>F11/D11</f>
+        <f t="shared" si="1"/>
         <v>59.660523122362761</v>
       </c>
       <c r="J11">
-        <f>G11/D11</f>
+        <f t="shared" si="2"/>
         <v>1.77441265811326</v>
       </c>
       <c r="K11">
-        <f>G11/E11</f>
+        <f t="shared" si="3"/>
         <v>0.25524188299909928</v>
       </c>
     </row>
@@ -8553,15 +9400,15 @@
         <v>54543.167999999998</v>
       </c>
       <c r="I12">
-        <f>F12/D12</f>
+        <f t="shared" si="1"/>
         <v>117.68715871679784</v>
       </c>
       <c r="J12">
-        <f>G12/D12</f>
+        <f t="shared" si="2"/>
         <v>1.5288265363711961</v>
       </c>
       <c r="K12">
-        <f>G12/E12</f>
+        <f t="shared" si="3"/>
         <v>0.21472396362270507</v>
       </c>
     </row>
@@ -8583,15 +9430,15 @@
         <v>100177.25</v>
       </c>
       <c r="I13">
-        <f>F13/D13</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J13">
-        <f>G13/D13</f>
+        <f t="shared" si="2"/>
         <v>1.3996294051795952</v>
       </c>
       <c r="K13">
-        <f>G13/E13</f>
+        <f t="shared" si="3"/>
         <v>0.19108633503496653</v>
       </c>
     </row>
@@ -8625,7 +9472,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView topLeftCell="A32" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
@@ -9057,8 +9904,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E51" sqref="E51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -9490,7 +10337,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:I12"/>
   <sheetViews>
-    <sheetView topLeftCell="A69" workbookViewId="0">
+    <sheetView topLeftCell="A33" workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
@@ -9766,7 +10613,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:I12"/>
   <sheetViews>
-    <sheetView topLeftCell="A35" workbookViewId="0">
+    <sheetView topLeftCell="A24" workbookViewId="0">
       <selection activeCell="O43" sqref="O43"/>
     </sheetView>
   </sheetViews>
@@ -10042,7 +10889,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:I11"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" workbookViewId="0">
+    <sheetView topLeftCell="A17" workbookViewId="0">
       <selection activeCell="I51" sqref="I51"/>
     </sheetView>
   </sheetViews>
@@ -10330,7 +11177,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:X17"/>
   <sheetViews>
-    <sheetView topLeftCell="A42" workbookViewId="0">
+    <sheetView topLeftCell="A30" workbookViewId="0">
       <selection activeCell="O27" sqref="O27"/>
     </sheetView>
   </sheetViews>
@@ -11313,10 +12160,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:P124"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="J60" sqref="J60"/>
+    <sheetView topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="L63" sqref="L63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -11706,6 +12553,671 @@
       <c r="H19">
         <f t="shared" si="0"/>
         <v>4.6754343147197854</v>
+      </c>
+    </row>
+    <row r="61" spans="4:16">
+      <c r="D61" t="s">
+        <v>51</v>
+      </c>
+      <c r="E61" t="s">
+        <v>52</v>
+      </c>
+      <c r="O61">
+        <v>107374</v>
+      </c>
+      <c r="P61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="4:16">
+      <c r="D62">
+        <v>0</v>
+      </c>
+      <c r="E62">
+        <v>3560709</v>
+      </c>
+      <c r="O62">
+        <v>93739</v>
+      </c>
+      <c r="P62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="4:16">
+      <c r="D63">
+        <v>1</v>
+      </c>
+      <c r="E63">
+        <v>409034</v>
+      </c>
+      <c r="O63">
+        <v>61732</v>
+      </c>
+      <c r="P63">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="64" spans="4:16">
+      <c r="D64">
+        <v>2</v>
+      </c>
+      <c r="E64">
+        <v>44542</v>
+      </c>
+      <c r="O64">
+        <v>32127</v>
+      </c>
+      <c r="P64">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="65" spans="4:16">
+      <c r="D65">
+        <v>3</v>
+      </c>
+      <c r="E65">
+        <v>13669</v>
+      </c>
+      <c r="O65">
+        <v>15557</v>
+      </c>
+      <c r="P65">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="66" spans="4:16">
+      <c r="D66">
+        <v>4</v>
+      </c>
+      <c r="E66">
+        <v>11480</v>
+      </c>
+      <c r="O66">
+        <v>7272</v>
+      </c>
+      <c r="P66">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="67" spans="4:16">
+      <c r="D67">
+        <v>5</v>
+      </c>
+      <c r="E67">
+        <v>11780</v>
+      </c>
+      <c r="O67">
+        <v>3753</v>
+      </c>
+      <c r="P67">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="68" spans="4:16">
+      <c r="D68">
+        <v>6</v>
+      </c>
+      <c r="E68">
+        <v>11422</v>
+      </c>
+      <c r="O68">
+        <v>1991</v>
+      </c>
+      <c r="P68">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="69" spans="4:16">
+      <c r="D69">
+        <v>7</v>
+      </c>
+      <c r="E69">
+        <v>10341</v>
+      </c>
+      <c r="H69" t="s">
+        <v>56</v>
+      </c>
+      <c r="O69">
+        <v>1156</v>
+      </c>
+      <c r="P69">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="70" spans="4:16">
+      <c r="D70">
+        <v>8</v>
+      </c>
+      <c r="E70">
+        <v>8518</v>
+      </c>
+      <c r="H70" t="s">
+        <v>57</v>
+      </c>
+      <c r="I70">
+        <v>6.1418600000000003</v>
+      </c>
+      <c r="O70">
+        <v>776</v>
+      </c>
+      <c r="P70">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="71" spans="4:16">
+      <c r="D71">
+        <v>9</v>
+      </c>
+      <c r="E71">
+        <v>6077</v>
+      </c>
+      <c r="H71" t="s">
+        <v>53</v>
+      </c>
+      <c r="I71">
+        <v>4.6806599999999996</v>
+      </c>
+      <c r="O71">
+        <v>566</v>
+      </c>
+      <c r="P71">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="72" spans="4:16">
+      <c r="D72">
+        <v>10</v>
+      </c>
+      <c r="E72">
+        <v>4037</v>
+      </c>
+      <c r="H72" t="s">
+        <v>54</v>
+      </c>
+      <c r="I72">
+        <v>1.8681399999999999</v>
+      </c>
+      <c r="O72">
+        <v>501</v>
+      </c>
+      <c r="P72">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="73" spans="4:16">
+      <c r="D73">
+        <v>11</v>
+      </c>
+      <c r="E73">
+        <v>2271</v>
+      </c>
+      <c r="H73" t="s">
+        <v>55</v>
+      </c>
+      <c r="I73">
+        <v>0.244141</v>
+      </c>
+      <c r="O73">
+        <v>378</v>
+      </c>
+      <c r="P73">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="74" spans="4:16">
+      <c r="D74">
+        <v>12</v>
+      </c>
+      <c r="E74">
+        <v>1190</v>
+      </c>
+      <c r="O74">
+        <v>345</v>
+      </c>
+      <c r="P74">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="75" spans="4:16">
+      <c r="D75">
+        <v>13</v>
+      </c>
+      <c r="E75">
+        <v>552</v>
+      </c>
+      <c r="O75">
+        <v>332</v>
+      </c>
+      <c r="P75">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="76" spans="4:16">
+      <c r="D76">
+        <v>14</v>
+      </c>
+      <c r="E76">
+        <v>243</v>
+      </c>
+      <c r="O76">
+        <v>329</v>
+      </c>
+      <c r="P76">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="77" spans="4:16">
+      <c r="D77">
+        <v>15</v>
+      </c>
+      <c r="E77">
+        <v>86</v>
+      </c>
+      <c r="O77">
+        <v>344</v>
+      </c>
+      <c r="P77">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="78" spans="4:16">
+      <c r="D78">
+        <v>16</v>
+      </c>
+      <c r="E78">
+        <v>38</v>
+      </c>
+      <c r="O78">
+        <v>327</v>
+      </c>
+      <c r="P78">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="79" spans="4:16">
+      <c r="D79">
+        <v>17</v>
+      </c>
+      <c r="E79">
+        <v>9</v>
+      </c>
+      <c r="O79">
+        <v>314</v>
+      </c>
+      <c r="P79">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="80" spans="4:16">
+      <c r="D80">
+        <v>19</v>
+      </c>
+      <c r="E80">
+        <v>1</v>
+      </c>
+      <c r="O80">
+        <v>339</v>
+      </c>
+      <c r="P80">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="81" spans="4:16">
+      <c r="D81">
+        <v>20</v>
+      </c>
+      <c r="E81">
+        <v>1</v>
+      </c>
+      <c r="O81">
+        <v>333</v>
+      </c>
+      <c r="P81">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="82" spans="4:16">
+      <c r="O82">
+        <v>314</v>
+      </c>
+      <c r="P82">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="83" spans="4:16">
+      <c r="O83">
+        <v>364</v>
+      </c>
+      <c r="P83">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="84" spans="4:16">
+      <c r="O84">
+        <v>341</v>
+      </c>
+      <c r="P84">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="85" spans="4:16">
+      <c r="O85">
+        <v>349</v>
+      </c>
+      <c r="P85">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="86" spans="4:16">
+      <c r="O86">
+        <v>366</v>
+      </c>
+      <c r="P86">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="87" spans="4:16">
+      <c r="O87">
+        <v>362</v>
+      </c>
+      <c r="P87">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="88" spans="4:16">
+      <c r="O88">
+        <v>364</v>
+      </c>
+      <c r="P88">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="89" spans="4:16">
+      <c r="O89">
+        <v>382</v>
+      </c>
+      <c r="P89">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="90" spans="4:16">
+      <c r="O90">
+        <v>420</v>
+      </c>
+      <c r="P90">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="91" spans="4:16">
+      <c r="O91">
+        <v>422</v>
+      </c>
+      <c r="P91">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="92" spans="4:16">
+      <c r="O92">
+        <v>542</v>
+      </c>
+      <c r="P92">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="93" spans="4:16">
+      <c r="O93">
+        <v>573</v>
+      </c>
+      <c r="P93">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="94" spans="4:16">
+      <c r="O94">
+        <v>607</v>
+      </c>
+      <c r="P94">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="95" spans="4:16">
+      <c r="O95">
+        <v>601</v>
+      </c>
+      <c r="P95">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="96" spans="4:16">
+      <c r="O96">
+        <v>641</v>
+      </c>
+      <c r="P96">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="97" spans="15:16">
+      <c r="O97">
+        <v>632</v>
+      </c>
+      <c r="P97">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="98" spans="15:16">
+      <c r="O98">
+        <v>647</v>
+      </c>
+      <c r="P98">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="99" spans="15:16">
+      <c r="O99">
+        <v>648</v>
+      </c>
+      <c r="P99">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="100" spans="15:16">
+      <c r="O100">
+        <v>644</v>
+      </c>
+      <c r="P100">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="101" spans="15:16">
+      <c r="O101">
+        <v>582</v>
+      </c>
+      <c r="P101">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="102" spans="15:16">
+      <c r="O102">
+        <v>562</v>
+      </c>
+      <c r="P102">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="103" spans="15:16">
+      <c r="O103">
+        <v>467</v>
+      </c>
+      <c r="P103">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="104" spans="15:16">
+      <c r="O104">
+        <v>442</v>
+      </c>
+      <c r="P104">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="105" spans="15:16">
+      <c r="O105">
+        <v>427</v>
+      </c>
+      <c r="P105">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="106" spans="15:16">
+      <c r="O106">
+        <v>360</v>
+      </c>
+      <c r="P106">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="107" spans="15:16">
+      <c r="O107">
+        <v>306</v>
+      </c>
+      <c r="P107">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="108" spans="15:16">
+      <c r="O108">
+        <v>254</v>
+      </c>
+      <c r="P108">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="109" spans="15:16">
+      <c r="O109">
+        <v>190</v>
+      </c>
+      <c r="P109">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="110" spans="15:16">
+      <c r="O110">
+        <v>153</v>
+      </c>
+      <c r="P110">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="111" spans="15:16">
+      <c r="O111">
+        <v>119</v>
+      </c>
+      <c r="P111">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="112" spans="15:16">
+      <c r="O112">
+        <v>91</v>
+      </c>
+      <c r="P112">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="113" spans="15:16">
+      <c r="O113">
+        <v>70</v>
+      </c>
+      <c r="P113">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="114" spans="15:16">
+      <c r="O114">
+        <v>40</v>
+      </c>
+      <c r="P114">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="115" spans="15:16">
+      <c r="O115">
+        <v>40</v>
+      </c>
+      <c r="P115">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="116" spans="15:16">
+      <c r="O116">
+        <v>29</v>
+      </c>
+      <c r="P116">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="117" spans="15:16">
+      <c r="O117">
+        <v>26</v>
+      </c>
+      <c r="P117">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="118" spans="15:16">
+      <c r="O118">
+        <v>21</v>
+      </c>
+      <c r="P118">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="119" spans="15:16">
+      <c r="O119">
+        <v>6</v>
+      </c>
+      <c r="P119">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="120" spans="15:16">
+      <c r="O120">
+        <v>3</v>
+      </c>
+      <c r="P120">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="121" spans="15:16">
+      <c r="O121">
+        <v>4</v>
+      </c>
+      <c r="P121">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="122" spans="15:16">
+      <c r="O122">
+        <v>2</v>
+      </c>
+      <c r="P122">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="123" spans="15:16">
+      <c r="O123">
+        <v>1</v>
+      </c>
+      <c r="P123">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="124" spans="15:16">
+      <c r="O124">
+        <v>1</v>
+      </c>
+      <c r="P124">
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -11728,7 +13240,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="M39" sqref="M39"/>
     </sheetView>
   </sheetViews>

</xml_diff>